<commit_message>
Check degli script + Realizzazione interfaccia update
</commit_message>
<xml_diff>
--- a/02_MySQL/running_time_analisys_aggiudicatari.xlsx
+++ b/02_MySQL/running_time_analisys_aggiudicatari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Documents\Programmazione\Github\BDT_Project_2021\02_MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDAA70B-0E99-4101-A84E-6C85A334731F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D4352C-9CEF-443F-A0E1-323DE9311F58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,40 +34,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Troncare una table di 50k righe</t>
-  </si>
-  <si>
-    <t>2 minuti 19 secondi</t>
-  </si>
-  <si>
-    <t>Retrieving di una tabella di 50k righe</t>
-  </si>
-  <si>
-    <t>Confronto con una nuova tabella di aggiudicatari, in cui:</t>
-  </si>
-  <si>
-    <t>Ipotetico problema</t>
-  </si>
-  <si>
-    <t>ha una crescita lineare</t>
-  </si>
-  <si>
-    <t>potrebbe non essere lineare (quasi sicuro)</t>
-  </si>
-  <si>
-    <t>- 50k aggiudicatari sono già presenti nel db</t>
-  </si>
-  <si>
-    <t>- 3k aggiudicatri sono nuovi aggiudicatari</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+  <si>
+    <t>Righe</t>
+  </si>
+  <si>
+    <t>Tempo</t>
+  </si>
+  <si>
+    <t>2 min, 19 sec</t>
+  </si>
+  <si>
+    <t>VERSIONE 1</t>
+  </si>
+  <si>
+    <t>VERSIONE 2</t>
+  </si>
+  <si>
+    <t>10 sec</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>Crescita lineare.</t>
+  </si>
+  <si>
+    <t>Crescita esponenziale.</t>
+  </si>
+  <si>
+    <t>50k</t>
+  </si>
+  <si>
+    <t>Valutazione Script per Update table elenco_aggiudicatari su MySQL</t>
+  </si>
+  <si>
+    <t>50k + 3k new</t>
+  </si>
+  <si>
+    <t>1M + 50k</t>
+  </si>
+  <si>
+    <t>2 min, 3 sec</t>
+  </si>
+  <si>
+    <t>o forse no…</t>
+  </si>
+  <si>
+    <t>52 min, 54 sec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,16 +96,83 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -92,14 +180,314 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -380,62 +768,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C5:L12"/>
+  <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="5.140625" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="5" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="8" width="20.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="L5" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="G3" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="G5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" t="s">
+      <c r="C6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L6" t="s">
+      <c r="D6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="G11" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="G12" s="2" t="s">
-        <v>8</v>
-      </c>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B3:E4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>